<commit_message>
Add Input event mask config
</commit_message>
<xml_diff>
--- a/doc/TIMER_UNIT_reference.xlsx
+++ b/doc/TIMER_UNIT_reference.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Info " sheetId="1" state="visible" r:id="rId2"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="197">
   <si>
     <t xml:space="preserve">Document Information</t>
   </si>
@@ -562,6 +562,14 @@
 - 1'b1: enabled</t>
   </si>
   <si>
+    <t xml:space="preserve">IEM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Timer low input event mask configuration bitfield:
+- 1'b0: disabled
+- 1'b1: enabled</t>
+  </si>
+  <si>
     <t xml:space="preserve">MODE</t>
   </si>
   <si>
@@ -620,6 +628,11 @@
   </si>
   <si>
     <t xml:space="preserve">Timer high compare match interrupt enable configuration bitfield:
+- 1'b0: disabled
+- 1'b1: enabled</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Timer high input event mask configuration bitfield:
 - 1'b0: disabled
 - 1'b1: enabled</t>
   </si>
@@ -1461,7 +1474,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="23.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="42.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="29.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="29.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="1" width="10.36"/>
   </cols>
   <sheetData>
@@ -2087,7 +2100,7 @@
   </sheetPr>
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -2136,7 +2149,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="35.73"/>
     <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="2" min="2" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="4.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="4.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="10.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="9"/>
@@ -2470,12 +2483,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H28"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="H15" activeCellId="0" sqref="H15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="H16" activeCellId="0" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2486,7 +2499,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="17.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="16.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="12.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="12.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="75.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="1" width="9"/>
   </cols>
@@ -2595,7 +2608,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="43.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="32.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>159</v>
       </c>
@@ -2603,7 +2616,7 @@
         <v>117</v>
       </c>
       <c r="C5" s="52" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D5" s="52" t="n">
         <v>1</v>
@@ -2621,7 +2634,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="43.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="43.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>161</v>
       </c>
@@ -2629,7 +2642,7 @@
         <v>117</v>
       </c>
       <c r="C6" s="52" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D6" s="52" t="n">
         <v>1</v>
@@ -2647,17 +2660,17 @@
         <v>162</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="43.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>163</v>
       </c>
       <c r="B7" s="56" t="s">
         <v>117</v>
       </c>
-      <c r="C7" s="61" t="n">
-        <v>6</v>
-      </c>
-      <c r="D7" s="61" t="n">
+      <c r="C7" s="52" t="n">
+        <v>5</v>
+      </c>
+      <c r="D7" s="52" t="n">
         <v>1</v>
       </c>
       <c r="E7" s="57" t="s">
@@ -2669,21 +2682,21 @@
       <c r="G7" s="60" t="s">
         <v>118</v>
       </c>
-      <c r="H7" s="62" t="s">
+      <c r="H7" s="58" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="43.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>165</v>
       </c>
       <c r="B8" s="56" t="s">
         <v>117</v>
       </c>
-      <c r="C8" s="52" t="n">
-        <v>7</v>
-      </c>
-      <c r="D8" s="52" t="n">
+      <c r="C8" s="61" t="n">
+        <v>6</v>
+      </c>
+      <c r="D8" s="61" t="n">
         <v>1</v>
       </c>
       <c r="E8" s="57" t="s">
@@ -2695,11 +2708,11 @@
       <c r="G8" s="60" t="s">
         <v>118</v>
       </c>
-      <c r="H8" s="58" t="s">
+      <c r="H8" s="62" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="43.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>167</v>
       </c>
@@ -2707,10 +2720,10 @@
         <v>117</v>
       </c>
       <c r="C9" s="52" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D9" s="52" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="E9" s="57" t="s">
         <v>120</v>
@@ -2725,7 +2738,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>169</v>
       </c>
@@ -2733,10 +2746,10 @@
         <v>117</v>
       </c>
       <c r="C10" s="52" t="n">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="D10" s="52" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="E10" s="57" t="s">
         <v>120</v>
@@ -2751,15 +2764,15 @@
         <v>170</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="43.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>153</v>
+        <v>171</v>
       </c>
       <c r="B11" s="56" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="C11" s="52" t="n">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="D11" s="52" t="n">
         <v>1</v>
@@ -2774,70 +2787,70 @@
         <v>118</v>
       </c>
       <c r="H11" s="58" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="43.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B12" s="56" t="s">
         <v>122</v>
       </c>
       <c r="C12" s="52" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D12" s="52" t="n">
         <v>1</v>
       </c>
       <c r="E12" s="57" t="s">
-        <v>172</v>
+        <v>120</v>
       </c>
       <c r="F12" s="52" t="s">
+        <v>120</v>
+      </c>
+      <c r="G12" s="60" t="s">
+        <v>118</v>
+      </c>
+      <c r="H12" s="58" t="s">
         <v>173</v>
       </c>
-      <c r="G12" s="60" t="s">
-        <v>118</v>
-      </c>
-      <c r="H12" s="58" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="43.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="13" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B13" s="56" t="s">
         <v>122</v>
       </c>
       <c r="C13" s="52" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D13" s="52" t="n">
         <v>1</v>
       </c>
       <c r="E13" s="57" t="s">
-        <v>120</v>
+        <v>174</v>
       </c>
       <c r="F13" s="52" t="s">
-        <v>120</v>
+        <v>175</v>
       </c>
       <c r="G13" s="60" t="s">
         <v>118</v>
       </c>
       <c r="H13" s="58" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="43.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="43.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B14" s="56" t="s">
         <v>122</v>
       </c>
       <c r="C14" s="52" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D14" s="52" t="n">
         <v>1</v>
@@ -2852,18 +2865,18 @@
         <v>118</v>
       </c>
       <c r="H14" s="58" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="43.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="32.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B15" s="56" t="s">
         <v>122</v>
       </c>
       <c r="C15" s="52" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D15" s="52" t="n">
         <v>1</v>
@@ -2878,20 +2891,20 @@
         <v>118</v>
       </c>
       <c r="H15" s="58" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="43.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="43.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B16" s="56" t="s">
         <v>122</v>
       </c>
-      <c r="C16" s="61" t="n">
-        <v>6</v>
-      </c>
-      <c r="D16" s="61" t="n">
+      <c r="C16" s="52" t="n">
+        <v>4</v>
+      </c>
+      <c r="D16" s="52" t="n">
         <v>1</v>
       </c>
       <c r="E16" s="57" t="s">
@@ -2903,19 +2916,19 @@
       <c r="G16" s="60" t="s">
         <v>118</v>
       </c>
-      <c r="H16" s="62" t="s">
-        <v>178</v>
+      <c r="H16" s="58" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="43.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>179</v>
+        <v>163</v>
       </c>
       <c r="B17" s="56" t="s">
         <v>122</v>
       </c>
       <c r="C17" s="52" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D17" s="52" t="n">
         <v>1</v>
@@ -2933,18 +2946,18 @@
         <v>180</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="43.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>125</v>
+        <v>165</v>
       </c>
       <c r="B18" s="56" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C18" s="61" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D18" s="61" t="n">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="E18" s="57" t="s">
         <v>120</v>
@@ -2955,22 +2968,22 @@
       <c r="G18" s="60" t="s">
         <v>118</v>
       </c>
-      <c r="H18" s="58" t="s">
+      <c r="H18" s="62" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="43.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>129</v>
+        <v>182</v>
       </c>
       <c r="B19" s="56" t="s">
-        <v>129</v>
-      </c>
-      <c r="C19" s="61" t="n">
-        <v>0</v>
-      </c>
-      <c r="D19" s="61" t="n">
-        <v>32</v>
+        <v>122</v>
+      </c>
+      <c r="C19" s="52" t="n">
+        <v>7</v>
+      </c>
+      <c r="D19" s="52" t="n">
+        <v>1</v>
       </c>
       <c r="E19" s="57" t="s">
         <v>120</v>
@@ -2982,15 +2995,15 @@
         <v>118</v>
       </c>
       <c r="H19" s="58" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="B20" s="56" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="C20" s="61" t="n">
         <v>0</v>
@@ -3008,15 +3021,15 @@
         <v>118</v>
       </c>
       <c r="H20" s="58" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B21" s="56" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="C21" s="61" t="n">
         <v>0</v>
@@ -3034,29 +3047,29 @@
         <v>118</v>
       </c>
       <c r="H21" s="58" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>185</v>
+        <v>132</v>
       </c>
       <c r="B22" s="56" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="C22" s="61" t="n">
         <v>0</v>
       </c>
       <c r="D22" s="61" t="n">
-        <v>1</v>
-      </c>
-      <c r="E22" s="61" t="s">
-        <v>172</v>
-      </c>
-      <c r="F22" s="61" t="s">
-        <v>173</v>
-      </c>
-      <c r="G22" s="61" t="s">
+        <v>32</v>
+      </c>
+      <c r="E22" s="57" t="s">
+        <v>120</v>
+      </c>
+      <c r="F22" s="52" t="s">
+        <v>120</v>
+      </c>
+      <c r="G22" s="60" t="s">
         <v>118</v>
       </c>
       <c r="H22" s="58" t="s">
@@ -3065,36 +3078,36 @@
     </row>
     <row r="23" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>187</v>
+        <v>135</v>
       </c>
       <c r="B23" s="56" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="C23" s="61" t="n">
         <v>0</v>
       </c>
       <c r="D23" s="61" t="n">
-        <v>1</v>
-      </c>
-      <c r="E23" s="61" t="s">
-        <v>172</v>
-      </c>
-      <c r="F23" s="61" t="s">
-        <v>173</v>
-      </c>
-      <c r="G23" s="61" t="s">
+        <v>32</v>
+      </c>
+      <c r="E23" s="57" t="s">
+        <v>120</v>
+      </c>
+      <c r="F23" s="52" t="s">
+        <v>120</v>
+      </c>
+      <c r="G23" s="60" t="s">
         <v>118</v>
       </c>
       <c r="H23" s="58" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B24" s="56" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="C24" s="61" t="n">
         <v>0</v>
@@ -3103,24 +3116,24 @@
         <v>1</v>
       </c>
       <c r="E24" s="61" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="F24" s="61" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="G24" s="61" t="s">
         <v>118</v>
       </c>
       <c r="H24" s="58" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B25" s="56" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="C25" s="61" t="n">
         <v>0</v>
@@ -3129,19 +3142,71 @@
         <v>1</v>
       </c>
       <c r="E25" s="61" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="F25" s="61" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="G25" s="61" t="s">
         <v>118</v>
       </c>
       <c r="H25" s="58" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="28" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+      <c r="B26" s="56" t="s">
+        <v>144</v>
+      </c>
+      <c r="C26" s="61" t="n">
+        <v>0</v>
+      </c>
+      <c r="D26" s="61" t="n">
+        <v>1</v>
+      </c>
+      <c r="E26" s="61" t="s">
+        <v>174</v>
+      </c>
+      <c r="F26" s="61" t="s">
+        <v>175</v>
+      </c>
+      <c r="G26" s="61" t="s">
+        <v>118</v>
+      </c>
+      <c r="H26" s="58" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B27" s="56" t="s">
+        <v>147</v>
+      </c>
+      <c r="C27" s="61" t="n">
+        <v>0</v>
+      </c>
+      <c r="D27" s="61" t="n">
+        <v>1</v>
+      </c>
+      <c r="E27" s="61" t="s">
+        <v>174</v>
+      </c>
+      <c r="F27" s="61" t="s">
+        <v>175</v>
+      </c>
+      <c r="G27" s="61" t="s">
+        <v>118</v>
+      </c>
+      <c r="H27" s="58" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -3180,7 +3245,7 @@
         <v>11</v>
       </c>
       <c r="C1" s="63" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="D1" s="63" t="s">
         <v>9</v>

</xml_diff>